<commit_message>
more iron in males
</commit_message>
<xml_diff>
--- a/data/data_alien-observational-untidy_20180310.xlsx
+++ b/data/data_alien-observational-untidy_20180310.xlsx
@@ -577,10 +577,10 @@
         <v>18.26</v>
       </c>
       <c r="I5">
-        <v>27.2</v>
+        <v>29.2</v>
       </c>
       <c r="J5">
-        <v>628</v>
+        <v>650</v>
       </c>
       <c r="K5">
         <v>123.552663781112</v>
@@ -749,10 +749,10 @@
         <v>17.89</v>
       </c>
       <c r="I9">
-        <v>25.2</v>
+        <v>27.2</v>
       </c>
       <c r="J9">
-        <v>536</v>
+        <v>558</v>
       </c>
       <c r="K9">
         <v>106.9705960935546</v>
@@ -835,10 +835,10 @@
         <v>15.03</v>
       </c>
       <c r="I11">
-        <v>22.7</v>
+        <v>24.7</v>
       </c>
       <c r="J11">
-        <v>432</v>
+        <v>454</v>
       </c>
       <c r="K11">
         <v>115.7305224152672</v>
@@ -878,10 +878,10 @@
         <v>20.22</v>
       </c>
       <c r="I12">
-        <v>25.8</v>
+        <v>27.8</v>
       </c>
       <c r="J12">
-        <v>595</v>
+        <v>617</v>
       </c>
       <c r="K12">
         <v>109.8634250511453</v>
@@ -921,10 +921,10 @@
         <v>16.28</v>
       </c>
       <c r="I13">
-        <v>23.7</v>
+        <v>25.7</v>
       </c>
       <c r="J13">
-        <v>405</v>
+        <v>427</v>
       </c>
       <c r="K13">
         <v>96.62067196580351</v>
@@ -1050,10 +1050,10 @@
         <v>18.59</v>
       </c>
       <c r="I16">
-        <v>25.9</v>
+        <v>27.9</v>
       </c>
       <c r="J16">
-        <v>488</v>
+        <v>510</v>
       </c>
       <c r="K16">
         <v>99.59438486856277</v>
@@ -1093,10 +1093,10 @@
         <v>15.23</v>
       </c>
       <c r="I17">
-        <v>25.1</v>
+        <v>27.1</v>
       </c>
       <c r="J17">
-        <v>477</v>
+        <v>499</v>
       </c>
       <c r="K17">
         <v>112.9227289256867</v>
@@ -1136,10 +1136,10 @@
         <v>15.26</v>
       </c>
       <c r="I18">
-        <v>24.9</v>
+        <v>26.9</v>
       </c>
       <c r="J18">
-        <v>479</v>
+        <v>501</v>
       </c>
       <c r="K18">
         <v>100.8504756749338</v>
@@ -1179,10 +1179,10 @@
         <v>18.42</v>
       </c>
       <c r="I19">
-        <v>23.8</v>
+        <v>25.8</v>
       </c>
       <c r="J19">
-        <v>448</v>
+        <v>470</v>
       </c>
       <c r="K19">
         <v>82.86850017859972</v>
@@ -1351,10 +1351,10 @@
         <v>17.11</v>
       </c>
       <c r="I23">
-        <v>23.7</v>
+        <v>25.7</v>
       </c>
       <c r="J23">
-        <v>518</v>
+        <v>540</v>
       </c>
       <c r="K23">
         <v>104.7177410134996</v>
@@ -1394,10 +1394,10 @@
         <v>15.28</v>
       </c>
       <c r="I24">
-        <v>24.6</v>
+        <v>26.6</v>
       </c>
       <c r="J24">
-        <v>469</v>
+        <v>491</v>
       </c>
       <c r="K24">
         <v>83.62997699067888</v>
@@ -1523,10 +1523,10 @@
         <v>17.12</v>
       </c>
       <c r="I27">
-        <v>22.4</v>
+        <v>24.4</v>
       </c>
       <c r="J27">
-        <v>411</v>
+        <v>433</v>
       </c>
       <c r="K27">
         <v>103.3906542389611</v>
@@ -1566,10 +1566,10 @@
         <v>18.14</v>
       </c>
       <c r="I28">
-        <v>25.2</v>
+        <v>27.2</v>
       </c>
       <c r="J28">
-        <v>545</v>
+        <v>567</v>
       </c>
       <c r="K28">
         <v>107.7708142220336</v>
@@ -1609,10 +1609,10 @@
         <v>13.21</v>
       </c>
       <c r="I29">
-        <v>23.7</v>
+        <v>25.7</v>
       </c>
       <c r="J29">
-        <v>458</v>
+        <v>480</v>
       </c>
       <c r="K29">
         <v>98.48830449428193</v>
@@ -1652,10 +1652,10 @@
         <v>20.51</v>
       </c>
       <c r="I30">
-        <v>26.5</v>
+        <v>28.5</v>
       </c>
       <c r="J30">
-        <v>701</v>
+        <v>723</v>
       </c>
       <c r="K30">
         <v>123.2198705117836</v>
@@ -1781,10 +1781,10 @@
         <v>18.31</v>
       </c>
       <c r="I33">
-        <v>20.6</v>
+        <v>22.6</v>
       </c>
       <c r="J33">
-        <v>362</v>
+        <v>384</v>
       </c>
       <c r="K33">
         <v>95.73236040575541</v>
@@ -1824,10 +1824,10 @@
         <v>15.17</v>
       </c>
       <c r="I34">
-        <v>25.8</v>
+        <v>27.8</v>
       </c>
       <c r="J34">
-        <v>511</v>
+        <v>533</v>
       </c>
       <c r="K34">
         <v>115.6482438124274</v>
@@ -1953,10 +1953,10 @@
         <v>15.67</v>
       </c>
       <c r="I37">
-        <v>24.3</v>
+        <v>26.3</v>
       </c>
       <c r="J37">
-        <v>550</v>
+        <v>572</v>
       </c>
       <c r="K37">
         <v>131.4543230674868</v>
@@ -1996,10 +1996,10 @@
         <v>16.83</v>
       </c>
       <c r="I38">
-        <v>25.6</v>
+        <v>27.6</v>
       </c>
       <c r="J38">
-        <v>537</v>
+        <v>559</v>
       </c>
       <c r="K38">
         <v>120.2108673807035</v>
@@ -2039,10 +2039,10 @@
         <v>17.34</v>
       </c>
       <c r="I39">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J39">
-        <v>661</v>
+        <v>683</v>
       </c>
       <c r="K39">
         <v>126.8720180038535</v>
@@ -2082,10 +2082,10 @@
         <v>16.22</v>
       </c>
       <c r="I40">
-        <v>23.8</v>
+        <v>25.8</v>
       </c>
       <c r="J40">
-        <v>435</v>
+        <v>457</v>
       </c>
       <c r="K40">
         <v>98.90256566301257</v>
@@ -2125,10 +2125,10 @@
         <v>17.03</v>
       </c>
       <c r="I41">
-        <v>25.7</v>
+        <v>27.7</v>
       </c>
       <c r="J41">
-        <v>563</v>
+        <v>585</v>
       </c>
       <c r="K41">
         <v>122.0398663954111</v>
@@ -2168,10 +2168,10 @@
         <v>15.71</v>
       </c>
       <c r="I42">
-        <v>21.1</v>
+        <v>23.1</v>
       </c>
       <c r="J42">
-        <v>400</v>
+        <v>422</v>
       </c>
       <c r="K42">
         <v>99.50440531220036</v>
@@ -2211,10 +2211,10 @@
         <v>22.06</v>
       </c>
       <c r="I43">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J43">
-        <v>759</v>
+        <v>781</v>
       </c>
       <c r="K43">
         <v>123.3519119774643</v>
@@ -2254,10 +2254,10 @@
         <v>18.97</v>
       </c>
       <c r="I44">
-        <v>24.4</v>
+        <v>26.4</v>
       </c>
       <c r="J44">
-        <v>461</v>
+        <v>483</v>
       </c>
       <c r="K44">
         <v>107.6354917396858</v>
@@ -2340,10 +2340,10 @@
         <v>17.08</v>
       </c>
       <c r="I46">
-        <v>23.8</v>
+        <v>25.8</v>
       </c>
       <c r="J46">
-        <v>439</v>
+        <v>461</v>
       </c>
       <c r="K46">
         <v>88.3818496412438</v>
@@ -2469,10 +2469,10 @@
         <v>14.05</v>
       </c>
       <c r="I49">
-        <v>21.8</v>
+        <v>23.8</v>
       </c>
       <c r="J49">
-        <v>372</v>
+        <v>394</v>
       </c>
       <c r="K49">
         <v>79.8399354929464</v>
@@ -2512,10 +2512,10 @@
         <v>22.67</v>
       </c>
       <c r="I50">
-        <v>26.7</v>
+        <v>28.7</v>
       </c>
       <c r="J50">
-        <v>902</v>
+        <v>924</v>
       </c>
       <c r="K50">
         <v>104.7516425626958</v>
@@ -2641,10 +2641,10 @@
         <v>18.63</v>
       </c>
       <c r="I53">
-        <v>23.2</v>
+        <v>25.2</v>
       </c>
       <c r="J53">
-        <v>542</v>
+        <v>564</v>
       </c>
       <c r="K53">
         <v>127.5899427939682</v>
@@ -2684,10 +2684,10 @@
         <v>16.23</v>
       </c>
       <c r="I54">
-        <v>22.9</v>
+        <v>24.9</v>
       </c>
       <c r="J54">
-        <v>384</v>
+        <v>406</v>
       </c>
       <c r="K54">
         <v>79.33910262427852</v>
@@ -2770,10 +2770,10 @@
         <v>17.07</v>
       </c>
       <c r="I56">
-        <v>23.2</v>
+        <v>25.2</v>
       </c>
       <c r="J56">
-        <v>388</v>
+        <v>410</v>
       </c>
       <c r="K56">
         <v>90.16007419880013</v>
@@ -2899,10 +2899,10 @@
         <v>16.73</v>
       </c>
       <c r="I59">
-        <v>22.6</v>
+        <v>24.6</v>
       </c>
       <c r="J59">
-        <v>406</v>
+        <v>428</v>
       </c>
       <c r="K59">
         <v>95.80780477309217</v>
@@ -2942,10 +2942,10 @@
         <v>12.51</v>
       </c>
       <c r="I60">
-        <v>21.7</v>
+        <v>23.7</v>
       </c>
       <c r="J60">
-        <v>382</v>
+        <v>404</v>
       </c>
       <c r="K60">
         <v>87.54498387522901</v>
@@ -2985,10 +2985,10 @@
         <v>21.34</v>
       </c>
       <c r="I61">
-        <v>25.7</v>
+        <v>27.7</v>
       </c>
       <c r="J61">
-        <v>599</v>
+        <v>621</v>
       </c>
       <c r="K61">
         <v>120.1530407366337</v>
@@ -3028,10 +3028,10 @@
         <v>20.23</v>
       </c>
       <c r="I62">
-        <v>24.4</v>
+        <v>26.4</v>
       </c>
       <c r="J62">
-        <v>490</v>
+        <v>512</v>
       </c>
       <c r="K62">
         <v>115.9407221621649</v>
@@ -3114,10 +3114,10 @@
         <v>16.93</v>
       </c>
       <c r="I64">
-        <v>24.2</v>
+        <v>26.2</v>
       </c>
       <c r="J64">
-        <v>486</v>
+        <v>508</v>
       </c>
       <c r="K64">
         <v>97.80454549331675</v>
@@ -3157,10 +3157,10 @@
         <v>15.25</v>
       </c>
       <c r="I65">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J65">
-        <v>441</v>
+        <v>463</v>
       </c>
       <c r="K65">
         <v>112.9332043267746</v>
@@ -3243,10 +3243,10 @@
         <v>15.81</v>
       </c>
       <c r="I67">
-        <v>23.5</v>
+        <v>25.5</v>
       </c>
       <c r="J67">
-        <v>420</v>
+        <v>442</v>
       </c>
       <c r="K67">
         <v>88.27017386731163</v>
@@ -3329,10 +3329,10 @@
         <v>16.97</v>
       </c>
       <c r="I69">
-        <v>22.2</v>
+        <v>24.2</v>
       </c>
       <c r="J69">
-        <v>405</v>
+        <v>427</v>
       </c>
       <c r="K69">
         <v>124.022611412151</v>
@@ -3458,10 +3458,10 @@
         <v>14.9</v>
       </c>
       <c r="I72">
-        <v>20.5</v>
+        <v>22.5</v>
       </c>
       <c r="J72">
-        <v>322</v>
+        <v>344</v>
       </c>
       <c r="K72">
         <v>74.38816831711904</v>
@@ -3544,10 +3544,10 @@
         <v>15.54</v>
       </c>
       <c r="I74">
-        <v>24.3</v>
+        <v>26.3</v>
       </c>
       <c r="J74">
-        <v>456</v>
+        <v>478</v>
       </c>
       <c r="K74">
         <v>107.9502919910552</v>
@@ -3587,10 +3587,10 @@
         <v>16.17</v>
       </c>
       <c r="I75">
-        <v>23.4</v>
+        <v>25.4</v>
       </c>
       <c r="J75">
-        <v>429</v>
+        <v>451</v>
       </c>
       <c r="K75">
         <v>107.7070655963154</v>
@@ -3759,10 +3759,10 @@
         <v>18.6</v>
       </c>
       <c r="I79">
-        <v>23.9</v>
+        <v>25.9</v>
       </c>
       <c r="J79">
-        <v>415</v>
+        <v>437</v>
       </c>
       <c r="K79">
         <v>103.0959800274986</v>
@@ -3802,10 +3802,10 @@
         <v>15.69</v>
       </c>
       <c r="I80">
-        <v>24.2</v>
+        <v>26.2</v>
       </c>
       <c r="J80">
-        <v>564</v>
+        <v>586</v>
       </c>
       <c r="K80">
         <v>125.4482198358335</v>
@@ -3888,10 +3888,10 @@
         <v>16.86</v>
       </c>
       <c r="I82">
-        <v>24.9</v>
+        <v>26.9</v>
       </c>
       <c r="J82">
-        <v>506</v>
+        <v>528</v>
       </c>
       <c r="K82">
         <v>124.7718812882291</v>
@@ -4017,10 +4017,10 @@
         <v>12.89</v>
       </c>
       <c r="I85">
-        <v>24.6</v>
+        <v>26.6</v>
       </c>
       <c r="J85">
-        <v>513</v>
+        <v>535</v>
       </c>
       <c r="K85">
         <v>119.8714816507999</v>
@@ -4447,10 +4447,10 @@
         <v>16.21</v>
       </c>
       <c r="I95">
-        <v>23.8</v>
+        <v>25.8</v>
       </c>
       <c r="J95">
-        <v>436</v>
+        <v>458</v>
       </c>
       <c r="K95">
         <v>91.65763890291571</v>
@@ -4490,10 +4490,10 @@
         <v>14.27</v>
       </c>
       <c r="I96">
-        <v>24.1</v>
+        <v>26.1</v>
       </c>
       <c r="J96">
-        <v>484</v>
+        <v>506</v>
       </c>
       <c r="K96">
         <v>99.46123397853955</v>
@@ -4576,10 +4576,10 @@
         <v>17.03</v>
       </c>
       <c r="I98">
-        <v>23.7</v>
+        <v>25.7</v>
       </c>
       <c r="J98">
-        <v>437</v>
+        <v>459</v>
       </c>
       <c r="K98">
         <v>106.9171529592841</v>
@@ -4748,10 +4748,10 @@
         <v>15.13</v>
       </c>
       <c r="I102">
-        <v>21.2</v>
+        <v>23.2</v>
       </c>
       <c r="J102">
-        <v>363</v>
+        <v>385</v>
       </c>
       <c r="K102">
         <v>93.15637108611531</v>
@@ -4834,10 +4834,10 @@
         <v>19.64</v>
       </c>
       <c r="I104">
-        <v>25.9</v>
+        <v>27.9</v>
       </c>
       <c r="J104">
-        <v>687</v>
+        <v>709</v>
       </c>
       <c r="K104">
         <v>120.029925664244</v>
@@ -4877,10 +4877,10 @@
         <v>17.4</v>
       </c>
       <c r="I105">
-        <v>27.8</v>
+        <v>29.8</v>
       </c>
       <c r="J105">
-        <v>783</v>
+        <v>805</v>
       </c>
       <c r="K105">
         <v>126.0622056218046</v>
@@ -4920,10 +4920,10 @@
         <v>20.38</v>
       </c>
       <c r="I106">
-        <v>24.7</v>
+        <v>26.7</v>
       </c>
       <c r="J106">
-        <v>629</v>
+        <v>651</v>
       </c>
       <c r="K106">
         <v>107.8428398542634</v>
@@ -4963,10 +4963,10 @@
         <v>15.54</v>
       </c>
       <c r="I107">
-        <v>23.1</v>
+        <v>25.1</v>
       </c>
       <c r="J107">
-        <v>437</v>
+        <v>459</v>
       </c>
       <c r="K107">
         <v>88.401830232791</v>
@@ -5006,10 +5006,10 @@
         <v>15.83</v>
       </c>
       <c r="I108">
-        <v>24.9</v>
+        <v>26.9</v>
       </c>
       <c r="J108">
-        <v>516</v>
+        <v>538</v>
       </c>
       <c r="K108">
         <v>109.673920831164</v>
@@ -5092,10 +5092,10 @@
         <v>16.51</v>
       </c>
       <c r="I110">
-        <v>24.7</v>
+        <v>26.7</v>
       </c>
       <c r="J110">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="K110">
         <v>115.5394907641775</v>
@@ -5307,10 +5307,10 @@
         <v>19.87</v>
       </c>
       <c r="I115">
-        <v>27.6</v>
+        <v>29.6</v>
       </c>
       <c r="J115">
-        <v>763</v>
+        <v>785</v>
       </c>
       <c r="K115">
         <v>128.5965591839618</v>
@@ -5350,10 +5350,10 @@
         <v>18.11</v>
       </c>
       <c r="I116">
-        <v>24.5</v>
+        <v>26.5</v>
       </c>
       <c r="J116">
-        <v>547</v>
+        <v>569</v>
       </c>
       <c r="K116">
         <v>131.7002009859528</v>
@@ -5565,10 +5565,10 @@
         <v>19.45</v>
       </c>
       <c r="I121">
-        <v>25.5</v>
+        <v>27.5</v>
       </c>
       <c r="J121">
-        <v>576</v>
+        <v>598</v>
       </c>
       <c r="K121">
         <v>110.7512165863235</v>
@@ -5608,10 +5608,10 @@
         <v>15.99</v>
       </c>
       <c r="I122">
-        <v>24.8</v>
+        <v>26.8</v>
       </c>
       <c r="J122">
-        <v>630</v>
+        <v>652</v>
       </c>
       <c r="K122">
         <v>139.4185605821156</v>
@@ -5651,10 +5651,10 @@
         <v>21.15</v>
       </c>
       <c r="I123">
-        <v>27.3</v>
+        <v>29.3</v>
       </c>
       <c r="J123">
-        <v>768</v>
+        <v>790</v>
       </c>
       <c r="K123">
         <v>133.2483703199</v>
@@ -5780,10 +5780,10 @@
         <v>15.79</v>
       </c>
       <c r="I126">
-        <v>25.7</v>
+        <v>27.7</v>
       </c>
       <c r="J126">
-        <v>604</v>
+        <v>626</v>
       </c>
       <c r="K126">
         <v>113.8830596648125</v>
@@ -5823,10 +5823,10 @@
         <v>16.94</v>
       </c>
       <c r="I127">
-        <v>24.4</v>
+        <v>26.4</v>
       </c>
       <c r="J127">
-        <v>454</v>
+        <v>476</v>
       </c>
       <c r="K127">
         <v>91.20696003986993</v>
@@ -5866,10 +5866,10 @@
         <v>16.82</v>
       </c>
       <c r="I128">
-        <v>25.2</v>
+        <v>27.2</v>
       </c>
       <c r="J128">
-        <v>573</v>
+        <v>595</v>
       </c>
       <c r="K128">
         <v>124.9642039139454</v>
@@ -5909,10 +5909,10 @@
         <v>19.46</v>
       </c>
       <c r="I129">
-        <v>23.8</v>
+        <v>25.8</v>
       </c>
       <c r="J129">
-        <v>556</v>
+        <v>578</v>
       </c>
       <c r="K129">
         <v>125.1027825742022</v>
@@ -5995,10 +5995,10 @@
         <v>14.78</v>
       </c>
       <c r="I131">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J131">
-        <v>399</v>
+        <v>421</v>
       </c>
       <c r="K131">
         <v>94.94435931444706</v>
@@ -6038,10 +6038,10 @@
         <v>18.06</v>
       </c>
       <c r="I132">
-        <v>25.7</v>
+        <v>27.7</v>
       </c>
       <c r="J132">
-        <v>609</v>
+        <v>631</v>
       </c>
       <c r="K132">
         <v>96.67742495920976</v>
@@ -6167,10 +6167,10 @@
         <v>14.13</v>
       </c>
       <c r="I135">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J135">
-        <v>481</v>
+        <v>503</v>
       </c>
       <c r="K135">
         <v>109.8185970702196</v>
@@ -6296,10 +6296,10 @@
         <v>18.48</v>
       </c>
       <c r="I138">
-        <v>23.9</v>
+        <v>25.9</v>
       </c>
       <c r="J138">
-        <v>432</v>
+        <v>454</v>
       </c>
       <c r="K138">
         <v>106.4798565528817</v>
@@ -6339,10 +6339,10 @@
         <v>16.76</v>
       </c>
       <c r="I139">
-        <v>22.6</v>
+        <v>24.6</v>
       </c>
       <c r="J139">
-        <v>424</v>
+        <v>446</v>
       </c>
       <c r="K139">
         <v>86.85426586368355</v>
@@ -6425,10 +6425,10 @@
         <v>16.36</v>
       </c>
       <c r="I141">
-        <v>22.7</v>
+        <v>24.7</v>
       </c>
       <c r="J141">
-        <v>366</v>
+        <v>388</v>
       </c>
       <c r="K141">
         <v>88.93164725837899</v>
@@ -6554,10 +6554,10 @@
         <v>20.18</v>
       </c>
       <c r="I144">
-        <v>25.4</v>
+        <v>27.4</v>
       </c>
       <c r="J144">
-        <v>525</v>
+        <v>547</v>
       </c>
       <c r="K144">
         <v>94.38647271037722</v>
@@ -6640,10 +6640,10 @@
         <v>17.18</v>
       </c>
       <c r="I146">
-        <v>26.2</v>
+        <v>28.2</v>
       </c>
       <c r="J146">
-        <v>657</v>
+        <v>679</v>
       </c>
       <c r="K146">
         <v>91.43188250114559</v>
@@ -6726,10 +6726,10 @@
         <v>17.3</v>
       </c>
       <c r="I148">
-        <v>26.1</v>
+        <v>28.1</v>
       </c>
       <c r="J148">
-        <v>507</v>
+        <v>529</v>
       </c>
       <c r="K148">
         <v>106.2385544333564</v>
@@ -6769,10 +6769,10 @@
         <v>11.99</v>
       </c>
       <c r="I149">
-        <v>24.4</v>
+        <v>26.4</v>
       </c>
       <c r="J149">
-        <v>449</v>
+        <v>471</v>
       </c>
       <c r="K149">
         <v>112.4967223289927</v>
@@ -6898,10 +6898,10 @@
         <v>12.9</v>
       </c>
       <c r="I152">
-        <v>23.1</v>
+        <v>25.1</v>
       </c>
       <c r="J152">
-        <v>442</v>
+        <v>464</v>
       </c>
       <c r="K152">
         <v>79.49957946791618</v>
@@ -6941,10 +6941,10 @@
         <v>19.77</v>
       </c>
       <c r="I153">
-        <v>25.5</v>
+        <v>27.5</v>
       </c>
       <c r="J153">
-        <v>627</v>
+        <v>649</v>
       </c>
       <c r="K153">
         <v>118.1566760247275</v>
@@ -7070,10 +7070,10 @@
         <v>17.16</v>
       </c>
       <c r="I156">
-        <v>26.4</v>
+        <v>28.4</v>
       </c>
       <c r="J156">
-        <v>613</v>
+        <v>635</v>
       </c>
       <c r="K156">
         <v>119.857624785935</v>
@@ -7113,10 +7113,10 @@
         <v>14.02</v>
       </c>
       <c r="I157">
-        <v>22.7</v>
+        <v>24.7</v>
       </c>
       <c r="J157">
-        <v>417</v>
+        <v>439</v>
       </c>
       <c r="K157">
         <v>98.41852394653456</v>
@@ -7285,10 +7285,10 @@
         <v>15.08</v>
       </c>
       <c r="I161">
-        <v>24.9</v>
+        <v>26.9</v>
       </c>
       <c r="J161">
-        <v>416</v>
+        <v>438</v>
       </c>
       <c r="K161">
         <v>93.2078067127746</v>
@@ -7328,10 +7328,10 @@
         <v>18.2</v>
       </c>
       <c r="I162">
-        <v>24.2</v>
+        <v>26.2</v>
       </c>
       <c r="J162">
-        <v>488</v>
+        <v>510</v>
       </c>
       <c r="K162">
         <v>121.3124771124866</v>
@@ -7371,10 +7371,10 @@
         <v>18.9</v>
       </c>
       <c r="I163">
-        <v>25.3</v>
+        <v>27.3</v>
       </c>
       <c r="J163">
-        <v>556</v>
+        <v>578</v>
       </c>
       <c r="K163">
         <v>110.3782989407625</v>
@@ -7414,10 +7414,10 @@
         <v>16.67</v>
       </c>
       <c r="I164">
-        <v>23.8</v>
+        <v>25.8</v>
       </c>
       <c r="J164">
-        <v>478</v>
+        <v>500</v>
       </c>
       <c r="K164">
         <v>122.9524798091893</v>
@@ -7500,10 +7500,10 @@
         <v>16.59</v>
       </c>
       <c r="I166">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J166">
-        <v>495</v>
+        <v>517</v>
       </c>
       <c r="K166">
         <v>121.1867777592998</v>
@@ -7543,10 +7543,10 @@
         <v>19.45</v>
       </c>
       <c r="I167">
-        <v>24.2</v>
+        <v>26.2</v>
       </c>
       <c r="J167">
-        <v>497</v>
+        <v>519</v>
       </c>
       <c r="K167">
         <v>107.003621300451</v>
@@ -7629,10 +7629,10 @@
         <v>16.95</v>
       </c>
       <c r="I169">
-        <v>22.3</v>
+        <v>24.3</v>
       </c>
       <c r="J169">
-        <v>433</v>
+        <v>455</v>
       </c>
       <c r="K169">
         <v>112.4693077221736</v>
@@ -7715,10 +7715,10 @@
         <v>17.49</v>
       </c>
       <c r="I171">
-        <v>24.9</v>
+        <v>26.9</v>
       </c>
       <c r="J171">
-        <v>483</v>
+        <v>505</v>
       </c>
       <c r="K171">
         <v>111.9641598249664</v>
@@ -7844,10 +7844,10 @@
         <v>15.52</v>
       </c>
       <c r="I174">
-        <v>24.4</v>
+        <v>26.4</v>
       </c>
       <c r="J174">
-        <v>466</v>
+        <v>488</v>
       </c>
       <c r="K174">
         <v>118.4267824040355</v>
@@ -7887,10 +7887,10 @@
         <v>18.39</v>
       </c>
       <c r="I175">
-        <v>26.2</v>
+        <v>28.2</v>
       </c>
       <c r="J175">
-        <v>526</v>
+        <v>548</v>
       </c>
       <c r="K175">
         <v>115.693917899512</v>
@@ -7930,10 +7930,10 @@
         <v>15.04</v>
       </c>
       <c r="I176">
-        <v>23.3</v>
+        <v>25.3</v>
       </c>
       <c r="J176">
-        <v>454</v>
+        <v>476</v>
       </c>
       <c r="K176">
         <v>105.9899595520217</v>
@@ -8016,10 +8016,10 @@
         <v>14.78</v>
       </c>
       <c r="I178">
-        <v>23.4</v>
+        <v>25.4</v>
       </c>
       <c r="J178">
-        <v>444</v>
+        <v>466</v>
       </c>
       <c r="K178">
         <v>120.7642439713867</v>
@@ -8059,10 +8059,10 @@
         <v>18.75</v>
       </c>
       <c r="I179">
-        <v>23.1</v>
+        <v>25.1</v>
       </c>
       <c r="J179">
-        <v>497</v>
+        <v>519</v>
       </c>
       <c r="K179">
         <v>126.8022802786432</v>
@@ -8102,10 +8102,10 @@
         <v>16.23</v>
       </c>
       <c r="I180">
-        <v>24.8</v>
+        <v>26.8</v>
       </c>
       <c r="J180">
-        <v>483</v>
+        <v>505</v>
       </c>
       <c r="K180">
         <v>113.3993663564009</v>
@@ -8145,10 +8145,10 @@
         <v>16.44</v>
       </c>
       <c r="I181">
-        <v>25.5</v>
+        <v>27.5</v>
       </c>
       <c r="J181">
-        <v>526</v>
+        <v>548</v>
       </c>
       <c r="K181">
         <v>109.2606362812524</v>
@@ -8188,10 +8188,10 @@
         <v>14.96</v>
       </c>
       <c r="I182">
-        <v>26.6</v>
+        <v>28.6</v>
       </c>
       <c r="J182">
-        <v>540</v>
+        <v>562</v>
       </c>
       <c r="K182">
         <v>110.7166109477485</v>
@@ -8403,10 +8403,10 @@
         <v>16.79</v>
       </c>
       <c r="I187">
-        <v>23.5</v>
+        <v>25.5</v>
       </c>
       <c r="J187">
-        <v>410</v>
+        <v>432</v>
       </c>
       <c r="K187">
         <v>102.3470672817232</v>
@@ -8446,10 +8446,10 @@
         <v>15.58</v>
       </c>
       <c r="I188">
-        <v>25.5</v>
+        <v>27.5</v>
       </c>
       <c r="J188">
-        <v>519</v>
+        <v>541</v>
       </c>
       <c r="K188">
         <v>128.8805842362826</v>
@@ -8489,10 +8489,10 @@
         <v>14.77</v>
       </c>
       <c r="I189">
-        <v>21.9</v>
+        <v>23.9</v>
       </c>
       <c r="J189">
-        <v>386</v>
+        <v>408</v>
       </c>
       <c r="K189">
         <v>97.87799879652427</v>
@@ -8575,10 +8575,10 @@
         <v>14.6</v>
       </c>
       <c r="I191">
-        <v>23.5</v>
+        <v>25.5</v>
       </c>
       <c r="J191">
-        <v>455</v>
+        <v>477</v>
       </c>
       <c r="K191">
         <v>88.97107308267142</v>
@@ -8618,10 +8618,10 @@
         <v>15.04</v>
       </c>
       <c r="I192">
-        <v>23.8</v>
+        <v>25.8</v>
       </c>
       <c r="J192">
-        <v>416</v>
+        <v>438</v>
       </c>
       <c r="K192">
         <v>97.70133299826914</v>
@@ -8704,10 +8704,10 @@
         <v>18.17</v>
       </c>
       <c r="I194">
-        <v>24.8</v>
+        <v>26.8</v>
       </c>
       <c r="J194">
-        <v>554</v>
+        <v>576</v>
       </c>
       <c r="K194">
         <v>144.1612515081512</v>
@@ -8790,10 +8790,10 @@
         <v>18.29</v>
       </c>
       <c r="I196">
-        <v>25.1</v>
+        <v>27.1</v>
       </c>
       <c r="J196">
-        <v>534</v>
+        <v>556</v>
       </c>
       <c r="K196">
         <v>126.7772592331318</v>
@@ -8919,10 +8919,10 @@
         <v>23.28</v>
       </c>
       <c r="I199">
-        <v>26.6</v>
+        <v>28.6</v>
       </c>
       <c r="J199">
-        <v>896</v>
+        <v>918</v>
       </c>
       <c r="K199">
         <v>124.545232332113</v>
@@ -9091,10 +9091,10 @@
         <v>18.81</v>
       </c>
       <c r="I203">
-        <v>25.4</v>
+        <v>27.4</v>
       </c>
       <c r="J203">
-        <v>572</v>
+        <v>594</v>
       </c>
       <c r="K203">
         <v>129.6536918990407</v>
@@ -9263,10 +9263,10 @@
         <v>19.11</v>
       </c>
       <c r="I207">
-        <v>25.6</v>
+        <v>27.6</v>
       </c>
       <c r="J207">
-        <v>594</v>
+        <v>616</v>
       </c>
       <c r="K207">
         <v>112.6998661923869</v>
@@ -9349,10 +9349,10 @@
         <v>14.56</v>
       </c>
       <c r="I209">
-        <v>24.5</v>
+        <v>26.5</v>
       </c>
       <c r="J209">
-        <v>447</v>
+        <v>469</v>
       </c>
       <c r="K209">
         <v>101.2652713411857</v>
@@ -9392,10 +9392,10 @@
         <v>17.4</v>
       </c>
       <c r="I210">
-        <v>23.8</v>
+        <v>25.8</v>
       </c>
       <c r="J210">
-        <v>480</v>
+        <v>502</v>
       </c>
       <c r="K210">
         <v>125.2612740056705</v>
@@ -9435,10 +9435,10 @@
         <v>15.62</v>
       </c>
       <c r="I211">
-        <v>23.1</v>
+        <v>25.1</v>
       </c>
       <c r="J211">
-        <v>457</v>
+        <v>479</v>
       </c>
       <c r="K211">
         <v>91.64958238423296</v>
@@ -9693,10 +9693,10 @@
         <v>13.74</v>
       </c>
       <c r="I217">
-        <v>24.7</v>
+        <v>26.7</v>
       </c>
       <c r="J217">
-        <v>430</v>
+        <v>452</v>
       </c>
       <c r="K217">
         <v>114.8554528345069</v>
@@ -9736,10 +9736,10 @@
         <v>20.13</v>
       </c>
       <c r="I218">
-        <v>24.2</v>
+        <v>26.2</v>
       </c>
       <c r="J218">
-        <v>517</v>
+        <v>539</v>
       </c>
       <c r="K218">
         <v>118.9983620252335</v>
@@ -9908,10 +9908,10 @@
         <v>14.06</v>
       </c>
       <c r="I222">
-        <v>23.8</v>
+        <v>25.8</v>
       </c>
       <c r="J222">
-        <v>401</v>
+        <v>423</v>
       </c>
       <c r="K222">
         <v>85.58506738307427</v>
@@ -9951,10 +9951,10 @@
         <v>15.82</v>
       </c>
       <c r="I223">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J223">
-        <v>472</v>
+        <v>494</v>
       </c>
       <c r="K223">
         <v>108.5645351650449</v>
@@ -9994,10 +9994,10 @@
         <v>18.88</v>
       </c>
       <c r="I224">
-        <v>26.5</v>
+        <v>28.5</v>
       </c>
       <c r="J224">
-        <v>672</v>
+        <v>694</v>
       </c>
       <c r="K224">
         <v>139.8062499692304</v>
@@ -10037,10 +10037,10 @@
         <v>17.74</v>
       </c>
       <c r="I225">
-        <v>24.5</v>
+        <v>26.5</v>
       </c>
       <c r="J225">
-        <v>488</v>
+        <v>510</v>
       </c>
       <c r="K225">
         <v>122.6741064538195</v>
@@ -10123,10 +10123,10 @@
         <v>15.56</v>
       </c>
       <c r="I227">
-        <v>23.7</v>
+        <v>25.7</v>
       </c>
       <c r="J227">
-        <v>418</v>
+        <v>440</v>
       </c>
       <c r="K227">
         <v>100.2319500333973</v>
@@ -10252,10 +10252,10 @@
         <v>17.52</v>
       </c>
       <c r="I230">
-        <v>24.1</v>
+        <v>26.1</v>
       </c>
       <c r="J230">
-        <v>420</v>
+        <v>442</v>
       </c>
       <c r="K230">
         <v>115.6383787124001</v>
@@ -10338,10 +10338,10 @@
         <v>15.36</v>
       </c>
       <c r="I232">
-        <v>22.6</v>
+        <v>24.6</v>
       </c>
       <c r="J232">
-        <v>423</v>
+        <v>445</v>
       </c>
       <c r="K232">
         <v>102.5182057825506</v>
@@ -10381,10 +10381,10 @@
         <v>20.01</v>
       </c>
       <c r="I233">
-        <v>23.6</v>
+        <v>25.6</v>
       </c>
       <c r="J233">
-        <v>486</v>
+        <v>508</v>
       </c>
       <c r="K233">
         <v>106.6532053716056</v>
@@ -10467,10 +10467,10 @@
         <v>15.97</v>
       </c>
       <c r="I235">
-        <v>24.6</v>
+        <v>26.6</v>
       </c>
       <c r="J235">
-        <v>496</v>
+        <v>518</v>
       </c>
       <c r="K235">
         <v>106.2685644507093</v>
@@ -10553,10 +10553,10 @@
         <v>17.7</v>
       </c>
       <c r="I237">
-        <v>24.9</v>
+        <v>26.9</v>
       </c>
       <c r="J237">
-        <v>539</v>
+        <v>561</v>
       </c>
       <c r="K237">
         <v>120.0948624678671</v>
@@ -10596,10 +10596,10 @@
         <v>20.34</v>
       </c>
       <c r="I238">
-        <v>24.6</v>
+        <v>26.6</v>
       </c>
       <c r="J238">
-        <v>611</v>
+        <v>633</v>
       </c>
       <c r="K238">
         <v>115.8483413642456</v>
@@ -10682,10 +10682,10 @@
         <v>15.05</v>
       </c>
       <c r="I240">
-        <v>23.1</v>
+        <v>25.1</v>
       </c>
       <c r="J240">
-        <v>425</v>
+        <v>447</v>
       </c>
       <c r="K240">
         <v>109.1298059736349</v>
@@ -10854,10 +10854,10 @@
         <v>16.39</v>
       </c>
       <c r="I244">
-        <v>21.4</v>
+        <v>23.4</v>
       </c>
       <c r="J244">
-        <v>411</v>
+        <v>433</v>
       </c>
       <c r="K244">
         <v>126.5890198935054</v>
@@ -10897,10 +10897,10 @@
         <v>14.91</v>
       </c>
       <c r="I245">
-        <v>25.3</v>
+        <v>27.3</v>
       </c>
       <c r="J245">
-        <v>492</v>
+        <v>514</v>
       </c>
       <c r="K245">
         <v>97.54731776912679</v>
@@ -10940,10 +10940,10 @@
         <v>16.73</v>
       </c>
       <c r="I246">
-        <v>24.2</v>
+        <v>26.2</v>
       </c>
       <c r="J246">
-        <v>464</v>
+        <v>486</v>
       </c>
       <c r="K246">
         <v>124.5751749786617</v>
@@ -11026,10 +11026,10 @@
         <v>14.39</v>
       </c>
       <c r="I248">
-        <v>23.7</v>
+        <v>25.7</v>
       </c>
       <c r="J248">
-        <v>463</v>
+        <v>485</v>
       </c>
       <c r="K248">
         <v>93.68829306767276</v>
@@ -11112,10 +11112,10 @@
         <v>14.43</v>
       </c>
       <c r="I250">
-        <v>24.7</v>
+        <v>26.7</v>
       </c>
       <c r="J250">
-        <v>427</v>
+        <v>449</v>
       </c>
       <c r="K250">
         <v>99.44771165225828</v>
@@ -11155,10 +11155,10 @@
         <v>14.29</v>
       </c>
       <c r="I251">
-        <v>23.9</v>
+        <v>25.9</v>
       </c>
       <c r="J251">
-        <v>444</v>
+        <v>466</v>
       </c>
       <c r="K251">
         <v>92.03972112177883</v>
@@ -11198,10 +11198,10 @@
         <v>14.13</v>
       </c>
       <c r="I252">
-        <v>24.1</v>
+        <v>26.1</v>
       </c>
       <c r="J252">
-        <v>467</v>
+        <v>489</v>
       </c>
       <c r="K252">
         <v>107.2484758455144</v>
@@ -11241,10 +11241,10 @@
         <v>19.05</v>
       </c>
       <c r="I253">
-        <v>22.5</v>
+        <v>24.5</v>
       </c>
       <c r="J253">
-        <v>380</v>
+        <v>402</v>
       </c>
       <c r="K253">
         <v>106.9141051806276</v>
@@ -11370,10 +11370,10 @@
         <v>13.99</v>
       </c>
       <c r="I256">
-        <v>23.9</v>
+        <v>25.9</v>
       </c>
       <c r="J256">
-        <v>402</v>
+        <v>424</v>
       </c>
       <c r="K256">
         <v>89.25830789292522</v>
@@ -11413,10 +11413,10 @@
         <v>18.7</v>
       </c>
       <c r="I257">
-        <v>24.3</v>
+        <v>26.3</v>
       </c>
       <c r="J257">
-        <v>522</v>
+        <v>544</v>
       </c>
       <c r="K257">
         <v>122.112555076483</v>
@@ -11456,10 +11456,10 @@
         <v>14.6</v>
       </c>
       <c r="I258">
-        <v>24.8</v>
+        <v>26.8</v>
       </c>
       <c r="J258">
-        <v>452</v>
+        <v>474</v>
       </c>
       <c r="K258">
         <v>113.1493005639853</v>
@@ -11499,10 +11499,10 @@
         <v>17.79</v>
       </c>
       <c r="I259">
-        <v>24.3</v>
+        <v>26.3</v>
       </c>
       <c r="J259">
-        <v>525</v>
+        <v>547</v>
       </c>
       <c r="K259">
         <v>99.11399010086834</v>
@@ -11628,10 +11628,10 @@
         <v>18.25</v>
       </c>
       <c r="I262">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J262">
-        <v>482</v>
+        <v>504</v>
       </c>
       <c r="K262">
         <v>128.7564074733615</v>
@@ -11800,10 +11800,10 @@
         <v>20.2</v>
       </c>
       <c r="I266">
-        <v>26.2</v>
+        <v>28.2</v>
       </c>
       <c r="J266">
-        <v>666</v>
+        <v>688</v>
       </c>
       <c r="K266">
         <v>111.7197371079977</v>
@@ -12015,10 +12015,10 @@
         <v>15.75</v>
       </c>
       <c r="I271">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J271">
-        <v>391</v>
+        <v>413</v>
       </c>
       <c r="K271">
         <v>109.8840994346845</v>
@@ -12101,10 +12101,10 @@
         <v>16.23</v>
       </c>
       <c r="I273">
-        <v>22.7</v>
+        <v>24.7</v>
       </c>
       <c r="J273">
-        <v>417</v>
+        <v>439</v>
       </c>
       <c r="K273">
         <v>105.0109907656305</v>
@@ -12273,10 +12273,10 @@
         <v>19.61</v>
       </c>
       <c r="I277">
-        <v>28.4</v>
+        <v>30.4</v>
       </c>
       <c r="J277">
-        <v>680</v>
+        <v>702</v>
       </c>
       <c r="K277">
         <v>115.1399701992164</v>
@@ -12617,10 +12617,10 @@
         <v>19.9</v>
       </c>
       <c r="I285">
-        <v>26.2</v>
+        <v>28.2</v>
       </c>
       <c r="J285">
-        <v>681</v>
+        <v>703</v>
       </c>
       <c r="K285">
         <v>104.2913484291562</v>
@@ -12660,10 +12660,10 @@
         <v>13.25</v>
       </c>
       <c r="I286">
-        <v>23.9</v>
+        <v>25.9</v>
       </c>
       <c r="J286">
-        <v>473</v>
+        <v>495</v>
       </c>
       <c r="K286">
         <v>111.3193173224799</v>
@@ -12703,10 +12703,10 @@
         <v>16.81</v>
       </c>
       <c r="I287">
-        <v>23.7</v>
+        <v>25.7</v>
       </c>
       <c r="J287">
-        <v>464</v>
+        <v>486</v>
       </c>
       <c r="K287">
         <v>117.4607713881293</v>
@@ -12746,10 +12746,10 @@
         <v>15.95</v>
       </c>
       <c r="I288">
-        <v>22.6</v>
+        <v>24.6</v>
       </c>
       <c r="J288">
-        <v>441</v>
+        <v>463</v>
       </c>
       <c r="K288">
         <v>112.5454326804269</v>
@@ -12789,10 +12789,10 @@
         <v>17.39</v>
       </c>
       <c r="I289">
-        <v>21.8</v>
+        <v>23.8</v>
       </c>
       <c r="J289">
-        <v>442</v>
+        <v>464</v>
       </c>
       <c r="K289">
         <v>98.7960909860001</v>
@@ -12961,10 +12961,10 @@
         <v>11.77</v>
       </c>
       <c r="I293">
-        <v>24.1</v>
+        <v>26.1</v>
       </c>
       <c r="J293">
-        <v>397</v>
+        <v>419</v>
       </c>
       <c r="K293">
         <v>78.77633729655199</v>
@@ -13047,10 +13047,10 @@
         <v>11.98</v>
       </c>
       <c r="I295">
-        <v>21.3</v>
+        <v>23.3</v>
       </c>
       <c r="J295">
-        <v>386</v>
+        <v>408</v>
       </c>
       <c r="K295">
         <v>107.4323645498269</v>
@@ -13090,10 +13090,10 @@
         <v>19.12</v>
       </c>
       <c r="I296">
-        <v>26.1</v>
+        <v>28.1</v>
       </c>
       <c r="J296">
-        <v>492</v>
+        <v>514</v>
       </c>
       <c r="K296">
         <v>93.38681864984883</v>
@@ -13133,10 +13133,10 @@
         <v>17.84</v>
       </c>
       <c r="I297">
-        <v>24.4</v>
+        <v>26.4</v>
       </c>
       <c r="J297">
-        <v>488</v>
+        <v>510</v>
       </c>
       <c r="K297">
         <v>110.1975857658318</v>
@@ -13219,10 +13219,10 @@
         <v>14.37</v>
       </c>
       <c r="I299">
-        <v>24.2</v>
+        <v>26.2</v>
       </c>
       <c r="J299">
-        <v>479</v>
+        <v>501</v>
       </c>
       <c r="K299">
         <v>94.89238345862695</v>
@@ -13262,10 +13262,10 @@
         <v>23.16</v>
       </c>
       <c r="I300">
-        <v>26.5</v>
+        <v>28.5</v>
       </c>
       <c r="J300">
-        <v>591</v>
+        <v>613</v>
       </c>
       <c r="K300">
         <v>121.5966216993567</v>
@@ -13305,10 +13305,10 @@
         <v>18.77</v>
       </c>
       <c r="I301">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J301">
-        <v>572</v>
+        <v>594</v>
       </c>
       <c r="K301">
         <v>123.5769936683265</v>
@@ -13348,10 +13348,10 @@
         <v>15.75</v>
       </c>
       <c r="I302">
-        <v>25.3</v>
+        <v>27.3</v>
       </c>
       <c r="J302">
-        <v>566</v>
+        <v>588</v>
       </c>
       <c r="K302">
         <v>142.8499890674627</v>
@@ -13434,10 +13434,10 @@
         <v>14.44</v>
       </c>
       <c r="I304">
-        <v>24.5</v>
+        <v>26.5</v>
       </c>
       <c r="J304">
-        <v>470</v>
+        <v>492</v>
       </c>
       <c r="K304">
         <v>120.6629444982011</v>
@@ -13477,10 +13477,10 @@
         <v>15.65</v>
       </c>
       <c r="I305">
-        <v>23.1</v>
+        <v>25.1</v>
       </c>
       <c r="J305">
-        <v>441</v>
+        <v>463</v>
       </c>
       <c r="K305">
         <v>94.14189871146125</v>
@@ -13520,10 +13520,10 @@
         <v>23.29</v>
       </c>
       <c r="I306">
-        <v>24.6</v>
+        <v>26.6</v>
       </c>
       <c r="J306">
-        <v>537</v>
+        <v>559</v>
       </c>
       <c r="K306">
         <v>121.0218520624533</v>
@@ -13563,10 +13563,10 @@
         <v>17.06</v>
       </c>
       <c r="I307">
-        <v>22.5</v>
+        <v>24.5</v>
       </c>
       <c r="J307">
-        <v>397</v>
+        <v>419</v>
       </c>
       <c r="K307">
         <v>82.01704724192899</v>
@@ -13606,10 +13606,10 @@
         <v>16.34</v>
       </c>
       <c r="I308">
-        <v>26.6</v>
+        <v>28.6</v>
       </c>
       <c r="J308">
-        <v>747</v>
+        <v>769</v>
       </c>
       <c r="K308">
         <v>126.5245053698146</v>
@@ -13649,10 +13649,10 @@
         <v>19.47</v>
       </c>
       <c r="I309">
-        <v>26.2</v>
+        <v>28.2</v>
       </c>
       <c r="J309">
-        <v>588</v>
+        <v>610</v>
       </c>
       <c r="K309">
         <v>122.1842910771333</v>
@@ -13821,10 +13821,10 @@
         <v>15.06</v>
       </c>
       <c r="I313">
-        <v>23.3</v>
+        <v>25.3</v>
       </c>
       <c r="J313">
-        <v>402</v>
+        <v>424</v>
       </c>
       <c r="K313">
         <v>84.03240593323018</v>
@@ -13907,10 +13907,10 @@
         <v>20.19</v>
       </c>
       <c r="I315">
-        <v>27.6</v>
+        <v>29.6</v>
       </c>
       <c r="J315">
-        <v>786</v>
+        <v>808</v>
       </c>
       <c r="K315">
         <v>117.5624247598458</v>
@@ -13950,10 +13950,10 @@
         <v>17.33</v>
       </c>
       <c r="I316">
-        <v>21.4</v>
+        <v>23.4</v>
       </c>
       <c r="J316">
-        <v>373</v>
+        <v>395</v>
       </c>
       <c r="K316">
         <v>111.6659328391433</v>
@@ -13993,10 +13993,10 @@
         <v>13.28</v>
       </c>
       <c r="I317">
-        <v>22.1</v>
+        <v>24.1</v>
       </c>
       <c r="J317">
-        <v>371</v>
+        <v>393</v>
       </c>
       <c r="K317">
         <v>96.56077889796654</v>
@@ -14036,10 +14036,10 @@
         <v>16.96</v>
       </c>
       <c r="I318">
-        <v>23.3</v>
+        <v>25.3</v>
       </c>
       <c r="J318">
-        <v>496</v>
+        <v>518</v>
       </c>
       <c r="K318">
         <v>114.3501297019036</v>
@@ -14122,10 +14122,10 @@
         <v>15.89</v>
       </c>
       <c r="I320">
-        <v>20.6</v>
+        <v>22.6</v>
       </c>
       <c r="J320">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="K320">
         <v>103.692530395292</v>
@@ -14165,10 +14165,10 @@
         <v>18.37</v>
       </c>
       <c r="I321">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J321">
-        <v>479</v>
+        <v>501</v>
       </c>
       <c r="K321">
         <v>102.5622168331483</v>
@@ -14208,10 +14208,10 @@
         <v>14.17</v>
       </c>
       <c r="I322">
-        <v>25.5</v>
+        <v>27.5</v>
       </c>
       <c r="J322">
-        <v>552</v>
+        <v>574</v>
       </c>
       <c r="K322">
         <v>82.09194332208466</v>
@@ -14251,10 +14251,10 @@
         <v>18.33</v>
       </c>
       <c r="I323">
-        <v>28.5</v>
+        <v>30.5</v>
       </c>
       <c r="J323">
-        <v>746</v>
+        <v>768</v>
       </c>
       <c r="K323">
         <v>120.3844799457629</v>
@@ -14423,10 +14423,10 @@
         <v>19.95</v>
       </c>
       <c r="I327">
-        <v>26.9</v>
+        <v>28.9</v>
       </c>
       <c r="J327">
-        <v>702</v>
+        <v>724</v>
       </c>
       <c r="K327">
         <v>110.4627230253523</v>
@@ -14466,10 +14466,10 @@
         <v>16.96</v>
       </c>
       <c r="I328">
-        <v>22.7</v>
+        <v>24.7</v>
       </c>
       <c r="J328">
-        <v>443</v>
+        <v>465</v>
       </c>
       <c r="K328">
         <v>109.4884884980871</v>
@@ -14509,10 +14509,10 @@
         <v>18.37</v>
       </c>
       <c r="I329">
-        <v>24.2</v>
+        <v>26.2</v>
       </c>
       <c r="J329">
-        <v>523</v>
+        <v>545</v>
       </c>
       <c r="K329">
         <v>129.3691955494594</v>
@@ -14638,10 +14638,10 @@
         <v>18.82</v>
       </c>
       <c r="I332">
-        <v>26.5</v>
+        <v>28.5</v>
       </c>
       <c r="J332">
-        <v>518</v>
+        <v>540</v>
       </c>
       <c r="K332">
         <v>104.9699718397948</v>
@@ -14724,10 +14724,10 @@
         <v>19.05</v>
       </c>
       <c r="I334">
-        <v>22.3</v>
+        <v>24.3</v>
       </c>
       <c r="J334">
-        <v>433</v>
+        <v>455</v>
       </c>
       <c r="K334">
         <v>108.470511564324</v>
@@ -14767,10 +14767,10 @@
         <v>14.41</v>
       </c>
       <c r="I335">
-        <v>21.4</v>
+        <v>23.4</v>
       </c>
       <c r="J335">
-        <v>370</v>
+        <v>392</v>
       </c>
       <c r="K335">
         <v>94.25933627611521</v>
@@ -14810,10 +14810,10 @@
         <v>13.14</v>
       </c>
       <c r="I336">
-        <v>23.5</v>
+        <v>25.5</v>
       </c>
       <c r="J336">
-        <v>402</v>
+        <v>424</v>
       </c>
       <c r="K336">
         <v>103.5941576847666</v>
@@ -14853,10 +14853,10 @@
         <v>17.3</v>
       </c>
       <c r="I337">
-        <v>22.8</v>
+        <v>24.8</v>
       </c>
       <c r="J337">
-        <v>402</v>
+        <v>424</v>
       </c>
       <c r="K337">
         <v>98.25957604462378</v>
@@ -14939,10 +14939,10 @@
         <v>18.32</v>
       </c>
       <c r="I339">
-        <v>28.3</v>
+        <v>30.3</v>
       </c>
       <c r="J339">
-        <v>663</v>
+        <v>685</v>
       </c>
       <c r="K339">
         <v>109.9951762367847</v>
@@ -15068,10 +15068,10 @@
         <v>15.96</v>
       </c>
       <c r="I342">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J342">
-        <v>454</v>
+        <v>476</v>
       </c>
       <c r="K342">
         <v>110.1698787562419</v>
@@ -15111,10 +15111,10 @@
         <v>18.55</v>
       </c>
       <c r="I343">
-        <v>25.1</v>
+        <v>27.1</v>
       </c>
       <c r="J343">
-        <v>580</v>
+        <v>602</v>
       </c>
       <c r="K343">
         <v>108.2868639002378</v>
@@ -15283,10 +15283,10 @@
         <v>18.25</v>
       </c>
       <c r="I347">
-        <v>24.2</v>
+        <v>26.2</v>
       </c>
       <c r="J347">
-        <v>547</v>
+        <v>569</v>
       </c>
       <c r="K347">
         <v>90.18864928362025</v>
@@ -15369,10 +15369,10 @@
         <v>21.55</v>
       </c>
       <c r="I349">
-        <v>27.6</v>
+        <v>29.6</v>
       </c>
       <c r="J349">
-        <v>752</v>
+        <v>774</v>
       </c>
       <c r="K349">
         <v>118.3037411882822</v>
@@ -15498,10 +15498,10 @@
         <v>13.66</v>
       </c>
       <c r="I352">
-        <v>23.6</v>
+        <v>25.6</v>
       </c>
       <c r="J352">
-        <v>445</v>
+        <v>467</v>
       </c>
       <c r="K352">
         <v>122.5461752871065</v>
@@ -15541,10 +15541,10 @@
         <v>11.51</v>
       </c>
       <c r="I353">
-        <v>24.7</v>
+        <v>26.7</v>
       </c>
       <c r="J353">
-        <v>476</v>
+        <v>498</v>
       </c>
       <c r="K353">
         <v>93.30743712702267</v>
@@ -15584,10 +15584,10 @@
         <v>12.49</v>
       </c>
       <c r="I354">
-        <v>24.6</v>
+        <v>26.6</v>
       </c>
       <c r="J354">
-        <v>512</v>
+        <v>534</v>
       </c>
       <c r="K354">
         <v>118.1555072995606</v>
@@ -15627,10 +15627,10 @@
         <v>16.88</v>
       </c>
       <c r="I355">
-        <v>25.9</v>
+        <v>27.9</v>
       </c>
       <c r="J355">
-        <v>527</v>
+        <v>549</v>
       </c>
       <c r="K355">
         <v>106.4194089572531</v>
@@ -15670,10 +15670,10 @@
         <v>20.74</v>
       </c>
       <c r="I356">
-        <v>26.4</v>
+        <v>28.4</v>
       </c>
       <c r="J356">
-        <v>738</v>
+        <v>760</v>
       </c>
       <c r="K356">
         <v>115.8973710377096</v>
@@ -15713,10 +15713,10 @@
         <v>14.64</v>
       </c>
       <c r="I357">
-        <v>23.3</v>
+        <v>25.3</v>
       </c>
       <c r="J357">
-        <v>429</v>
+        <v>451</v>
       </c>
       <c r="K357">
         <v>98.53540649799243</v>
@@ -15971,10 +15971,10 @@
         <v>17.99</v>
       </c>
       <c r="I363">
-        <v>26.1</v>
+        <v>28.1</v>
       </c>
       <c r="J363">
-        <v>562</v>
+        <v>584</v>
       </c>
       <c r="K363">
         <v>126.6012919630831</v>
@@ -16186,10 +16186,10 @@
         <v>14.31</v>
       </c>
       <c r="I368">
-        <v>23.6</v>
+        <v>25.6</v>
       </c>
       <c r="J368">
-        <v>455</v>
+        <v>477</v>
       </c>
       <c r="K368">
         <v>112.7151447292656</v>
@@ -16315,10 +16315,10 @@
         <v>20.25</v>
       </c>
       <c r="I371">
-        <v>26.3</v>
+        <v>28.3</v>
       </c>
       <c r="J371">
-        <v>718</v>
+        <v>740</v>
       </c>
       <c r="K371">
         <v>123.0233821336558</v>
@@ -16444,10 +16444,10 @@
         <v>19.9</v>
       </c>
       <c r="I374">
-        <v>23.9</v>
+        <v>25.9</v>
       </c>
       <c r="J374">
-        <v>473</v>
+        <v>495</v>
       </c>
       <c r="K374">
         <v>98.90053795669516</v>
@@ -16530,10 +16530,10 @@
         <v>18.98</v>
       </c>
       <c r="I376">
-        <v>24.5</v>
+        <v>26.5</v>
       </c>
       <c r="J376">
-        <v>513</v>
+        <v>535</v>
       </c>
       <c r="K376">
         <v>113.5629344381893</v>
@@ -16573,10 +16573,10 @@
         <v>16.46</v>
       </c>
       <c r="I377">
-        <v>22.8</v>
+        <v>24.8</v>
       </c>
       <c r="J377">
-        <v>458</v>
+        <v>480</v>
       </c>
       <c r="K377">
         <v>128.4909249533885</v>
@@ -16616,10 +16616,10 @@
         <v>14.09</v>
       </c>
       <c r="I378">
-        <v>22.3</v>
+        <v>24.3</v>
       </c>
       <c r="J378">
-        <v>421</v>
+        <v>443</v>
       </c>
       <c r="K378">
         <v>108.4756752497243</v>
@@ -16788,10 +16788,10 @@
         <v>21.95</v>
       </c>
       <c r="I382">
-        <v>23.4</v>
+        <v>25.4</v>
       </c>
       <c r="J382">
-        <v>440</v>
+        <v>462</v>
       </c>
       <c r="K382">
         <v>102.8021833298088</v>
@@ -16831,10 +16831,10 @@
         <v>13.34</v>
       </c>
       <c r="I383">
-        <v>23.7</v>
+        <v>25.7</v>
       </c>
       <c r="J383">
-        <v>456</v>
+        <v>478</v>
       </c>
       <c r="K383">
         <v>91.57384696284151</v>
@@ -17132,10 +17132,10 @@
         <v>23.3</v>
       </c>
       <c r="I390">
-        <v>28.2</v>
+        <v>30.2</v>
       </c>
       <c r="J390">
-        <v>808</v>
+        <v>830</v>
       </c>
       <c r="K390">
         <v>119.2290007741432</v>
@@ -17347,10 +17347,10 @@
         <v>14.76</v>
       </c>
       <c r="I395">
-        <v>22.5</v>
+        <v>24.5</v>
       </c>
       <c r="J395">
-        <v>478</v>
+        <v>500</v>
       </c>
       <c r="K395">
         <v>105.7092237330416</v>
@@ -17390,10 +17390,10 @@
         <v>19.78</v>
       </c>
       <c r="I396">
-        <v>23.1</v>
+        <v>25.1</v>
       </c>
       <c r="J396">
-        <v>484</v>
+        <v>506</v>
       </c>
       <c r="K396">
         <v>100.1475520376871</v>
@@ -17433,10 +17433,10 @@
         <v>18.55</v>
       </c>
       <c r="I397">
-        <v>21.1</v>
+        <v>23.1</v>
       </c>
       <c r="J397">
-        <v>376</v>
+        <v>398</v>
       </c>
       <c r="K397">
         <v>79.11700948927856</v>
@@ -17476,10 +17476,10 @@
         <v>13.27</v>
       </c>
       <c r="I398">
-        <v>24.1</v>
+        <v>26.1</v>
       </c>
       <c r="J398">
-        <v>464</v>
+        <v>486</v>
       </c>
       <c r="K398">
         <v>115.5361212721415</v>
@@ -17605,10 +17605,10 @@
         <v>14.35</v>
       </c>
       <c r="I401">
-        <v>23.4</v>
+        <v>25.4</v>
       </c>
       <c r="J401">
-        <v>466</v>
+        <v>488</v>
       </c>
       <c r="K401">
         <v>111.6543891130796</v>
@@ -17648,10 +17648,10 @@
         <v>14.08</v>
       </c>
       <c r="I402">
-        <v>22.7</v>
+        <v>24.7</v>
       </c>
       <c r="J402">
-        <v>377</v>
+        <v>399</v>
       </c>
       <c r="K402">
         <v>86.96062175514035</v>
@@ -17691,10 +17691,10 @@
         <v>17.69</v>
       </c>
       <c r="I403">
-        <v>24.4</v>
+        <v>26.4</v>
       </c>
       <c r="J403">
-        <v>470</v>
+        <v>492</v>
       </c>
       <c r="K403">
         <v>121.0099300591582</v>
@@ -17734,10 +17734,10 @@
         <v>16.23</v>
       </c>
       <c r="I404">
-        <v>26.5</v>
+        <v>28.5</v>
       </c>
       <c r="J404">
-        <v>644</v>
+        <v>666</v>
       </c>
       <c r="K404">
         <v>108.6014280997401</v>
@@ -17777,10 +17777,10 @@
         <v>17.95</v>
       </c>
       <c r="I405">
-        <v>23.6</v>
+        <v>25.6</v>
       </c>
       <c r="J405">
-        <v>506</v>
+        <v>528</v>
       </c>
       <c r="K405">
         <v>112.541328933366</v>
@@ -17820,10 +17820,10 @@
         <v>20.15</v>
       </c>
       <c r="I406">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J406">
-        <v>625</v>
+        <v>647</v>
       </c>
       <c r="K406">
         <v>125.4936699127699</v>
@@ -17863,10 +17863,10 @@
         <v>20.66</v>
       </c>
       <c r="I407">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J407">
-        <v>490</v>
+        <v>512</v>
       </c>
       <c r="K407">
         <v>106.9786663694243</v>
@@ -17906,10 +17906,10 @@
         <v>16.4</v>
       </c>
       <c r="I408">
-        <v>22.3</v>
+        <v>24.3</v>
       </c>
       <c r="J408">
-        <v>429</v>
+        <v>451</v>
       </c>
       <c r="K408">
         <v>121.8738840538911</v>
@@ -17949,10 +17949,10 @@
         <v>16.48</v>
       </c>
       <c r="I409">
-        <v>24.6</v>
+        <v>26.6</v>
       </c>
       <c r="J409">
-        <v>553</v>
+        <v>575</v>
       </c>
       <c r="K409">
         <v>124.010502821868</v>
@@ -17992,10 +17992,10 @@
         <v>16.46</v>
       </c>
       <c r="I410">
-        <v>20.1</v>
+        <v>22.1</v>
       </c>
       <c r="J410">
-        <v>333</v>
+        <v>355</v>
       </c>
       <c r="K410">
         <v>75.82031994124364</v>
@@ -18207,10 +18207,10 @@
         <v>18.99</v>
       </c>
       <c r="I415">
-        <v>25.8</v>
+        <v>27.8</v>
       </c>
       <c r="J415">
-        <v>567</v>
+        <v>589</v>
       </c>
       <c r="K415">
         <v>104.3230623009731</v>
@@ -18250,10 +18250,10 @@
         <v>19.26</v>
       </c>
       <c r="I416">
-        <v>23.1</v>
+        <v>25.1</v>
       </c>
       <c r="J416">
-        <v>431</v>
+        <v>453</v>
       </c>
       <c r="K416">
         <v>117.6801553771436</v>
@@ -18336,10 +18336,10 @@
         <v>23.82</v>
       </c>
       <c r="I418">
-        <v>25.2</v>
+        <v>27.2</v>
       </c>
       <c r="J418">
-        <v>650</v>
+        <v>672</v>
       </c>
       <c r="K418">
         <v>142.9093930299958</v>
@@ -18422,10 +18422,10 @@
         <v>15.43</v>
       </c>
       <c r="I420">
-        <v>24.8</v>
+        <v>26.8</v>
       </c>
       <c r="J420">
-        <v>513</v>
+        <v>535</v>
       </c>
       <c r="K420">
         <v>112.0785245146204</v>
@@ -18465,10 +18465,10 @@
         <v>18.9</v>
       </c>
       <c r="I421">
-        <v>24.3</v>
+        <v>26.3</v>
       </c>
       <c r="J421">
-        <v>509</v>
+        <v>531</v>
       </c>
       <c r="K421">
         <v>121.6671180606316</v>
@@ -18852,10 +18852,10 @@
         <v>18.77</v>
       </c>
       <c r="I430">
-        <v>24.8</v>
+        <v>26.8</v>
       </c>
       <c r="J430">
-        <v>474</v>
+        <v>496</v>
       </c>
       <c r="K430">
         <v>95.9721908065443</v>
@@ -18895,10 +18895,10 @@
         <v>16.61</v>
       </c>
       <c r="I431">
-        <v>26.5</v>
+        <v>28.5</v>
       </c>
       <c r="J431">
-        <v>539</v>
+        <v>561</v>
       </c>
       <c r="K431">
         <v>104.2554861534835</v>
@@ -18938,10 +18938,10 @@
         <v>21.64</v>
       </c>
       <c r="I432">
-        <v>26.2</v>
+        <v>28.2</v>
       </c>
       <c r="J432">
-        <v>568</v>
+        <v>590</v>
       </c>
       <c r="K432">
         <v>117.2838552104158</v>
@@ -19024,10 +19024,10 @@
         <v>16.37</v>
       </c>
       <c r="I434">
-        <v>24.1</v>
+        <v>26.1</v>
       </c>
       <c r="J434">
-        <v>501</v>
+        <v>523</v>
       </c>
       <c r="K434">
         <v>91.96847361353232</v>
@@ -19067,10 +19067,10 @@
         <v>17.02</v>
       </c>
       <c r="I435">
-        <v>22.4</v>
+        <v>24.4</v>
       </c>
       <c r="J435">
-        <v>421</v>
+        <v>443</v>
       </c>
       <c r="K435">
         <v>107.2587997592747</v>
@@ -19110,10 +19110,10 @@
         <v>19.86</v>
       </c>
       <c r="I436">
-        <v>23.9</v>
+        <v>25.9</v>
       </c>
       <c r="J436">
-        <v>513</v>
+        <v>535</v>
       </c>
       <c r="K436">
         <v>117.3771955367029</v>
@@ -19153,10 +19153,10 @@
         <v>14.22</v>
       </c>
       <c r="I437">
-        <v>22.9</v>
+        <v>24.9</v>
       </c>
       <c r="J437">
-        <v>414</v>
+        <v>436</v>
       </c>
       <c r="K437">
         <v>102.8123498019621</v>
@@ -19239,10 +19239,10 @@
         <v>15.62</v>
       </c>
       <c r="I439">
-        <v>23.9</v>
+        <v>25.9</v>
       </c>
       <c r="J439">
-        <v>445</v>
+        <v>467</v>
       </c>
       <c r="K439">
         <v>122.4199864950546</v>
@@ -19282,10 +19282,10 @@
         <v>23.57</v>
       </c>
       <c r="I440">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J440">
-        <v>686</v>
+        <v>708</v>
       </c>
       <c r="K440">
         <v>101.6998087795967</v>
@@ -19325,10 +19325,10 @@
         <v>15.87</v>
       </c>
       <c r="I441">
-        <v>23.3</v>
+        <v>25.3</v>
       </c>
       <c r="J441">
-        <v>493</v>
+        <v>515</v>
       </c>
       <c r="K441">
         <v>118.2353341143988</v>
@@ -19368,10 +19368,10 @@
         <v>16.89</v>
       </c>
       <c r="I442">
-        <v>22.3</v>
+        <v>24.3</v>
       </c>
       <c r="J442">
-        <v>403</v>
+        <v>425</v>
       </c>
       <c r="K442">
         <v>110.6969803327367</v>
@@ -19411,10 +19411,10 @@
         <v>15.08</v>
       </c>
       <c r="I443">
-        <v>24.5</v>
+        <v>26.5</v>
       </c>
       <c r="J443">
-        <v>543</v>
+        <v>565</v>
       </c>
       <c r="K443">
         <v>121.4683023977389</v>
@@ -19454,10 +19454,10 @@
         <v>14.51</v>
       </c>
       <c r="I444">
-        <v>22.1</v>
+        <v>24.1</v>
       </c>
       <c r="J444">
-        <v>463</v>
+        <v>485</v>
       </c>
       <c r="K444">
         <v>108.4341501632463</v>
@@ -19583,10 +19583,10 @@
         <v>19.78</v>
       </c>
       <c r="I447">
-        <v>23.1</v>
+        <v>25.1</v>
       </c>
       <c r="J447">
-        <v>444</v>
+        <v>466</v>
       </c>
       <c r="K447">
         <v>100.8820202113585</v>
@@ -19798,10 +19798,10 @@
         <v>20.1</v>
       </c>
       <c r="I452">
-        <v>24.9</v>
+        <v>26.9</v>
       </c>
       <c r="J452">
-        <v>628</v>
+        <v>650</v>
       </c>
       <c r="K452">
         <v>127.2462259037318</v>
@@ -20357,10 +20357,10 @@
         <v>15.09</v>
       </c>
       <c r="I465">
-        <v>23.7</v>
+        <v>25.7</v>
       </c>
       <c r="J465">
-        <v>472</v>
+        <v>494</v>
       </c>
       <c r="K465">
         <v>102.9753065303802</v>
@@ -20400,10 +20400,10 @@
         <v>19.48</v>
       </c>
       <c r="I466">
-        <v>23.9</v>
+        <v>25.9</v>
       </c>
       <c r="J466">
-        <v>446</v>
+        <v>468</v>
       </c>
       <c r="K466">
         <v>125.1423681970537</v>
@@ -20529,10 +20529,10 @@
         <v>16.66</v>
       </c>
       <c r="I469">
-        <v>22.8</v>
+        <v>24.8</v>
       </c>
       <c r="J469">
-        <v>472</v>
+        <v>494</v>
       </c>
       <c r="K469">
         <v>84.13274235511906</v>
@@ -20572,10 +20572,10 @@
         <v>13.99</v>
       </c>
       <c r="I470">
-        <v>24.2</v>
+        <v>26.2</v>
       </c>
       <c r="J470">
-        <v>454</v>
+        <v>476</v>
       </c>
       <c r="K470">
         <v>108.9544209991529</v>
@@ -20701,10 +20701,10 @@
         <v>18.76</v>
       </c>
       <c r="I473">
-        <v>24.8</v>
+        <v>26.8</v>
       </c>
       <c r="J473">
-        <v>511</v>
+        <v>533</v>
       </c>
       <c r="K473">
         <v>109.6747114266566</v>
@@ -20744,10 +20744,10 @@
         <v>14.15</v>
       </c>
       <c r="I474">
-        <v>24.4</v>
+        <v>26.4</v>
       </c>
       <c r="J474">
-        <v>599</v>
+        <v>621</v>
       </c>
       <c r="K474">
         <v>107.7281236154322</v>
@@ -20873,10 +20873,10 @@
         <v>24.57</v>
       </c>
       <c r="I477">
-        <v>27.5</v>
+        <v>29.5</v>
       </c>
       <c r="J477">
-        <v>852</v>
+        <v>874</v>
       </c>
       <c r="K477">
         <v>112.6157029512685</v>
@@ -21002,10 +21002,10 @@
         <v>14.12</v>
       </c>
       <c r="I480">
-        <v>22.6</v>
+        <v>24.6</v>
       </c>
       <c r="J480">
-        <v>498</v>
+        <v>520</v>
       </c>
       <c r="K480">
         <v>109.5658965443534</v>
@@ -21045,10 +21045,10 @@
         <v>15.16</v>
       </c>
       <c r="I481">
-        <v>22.5</v>
+        <v>24.5</v>
       </c>
       <c r="J481">
-        <v>379</v>
+        <v>401</v>
       </c>
       <c r="K481">
         <v>80.53226953976953</v>
@@ -21303,10 +21303,10 @@
         <v>13.7</v>
       </c>
       <c r="I487">
-        <v>18.9</v>
+        <v>20.9</v>
       </c>
       <c r="J487">
-        <v>321</v>
+        <v>343</v>
       </c>
       <c r="K487">
         <v>85.1588142167929</v>
@@ -21346,10 +21346,10 @@
         <v>15.45</v>
       </c>
       <c r="I488">
-        <v>22.3</v>
+        <v>24.3</v>
       </c>
       <c r="J488">
-        <v>357</v>
+        <v>379</v>
       </c>
       <c r="K488">
         <v>79.04265625989139</v>
@@ -21389,10 +21389,10 @@
         <v>17.7</v>
       </c>
       <c r="I489">
-        <v>24.3</v>
+        <v>26.3</v>
       </c>
       <c r="J489">
-        <v>533</v>
+        <v>555</v>
       </c>
       <c r="K489">
         <v>109.6487085606077</v>
@@ -21432,10 +21432,10 @@
         <v>17.06</v>
       </c>
       <c r="I490">
-        <v>26.3</v>
+        <v>28.3</v>
       </c>
       <c r="J490">
-        <v>611</v>
+        <v>633</v>
       </c>
       <c r="K490">
         <v>106.0323043222926</v>
@@ -21604,10 +21604,10 @@
         <v>20.91</v>
       </c>
       <c r="I494">
-        <v>23.8</v>
+        <v>25.8</v>
       </c>
       <c r="J494">
-        <v>481</v>
+        <v>503</v>
       </c>
       <c r="K494">
         <v>102.9030325912976</v>
@@ -21647,10 +21647,10 @@
         <v>18.69</v>
       </c>
       <c r="I495">
-        <v>23.9</v>
+        <v>25.9</v>
       </c>
       <c r="J495">
-        <v>453</v>
+        <v>475</v>
       </c>
       <c r="K495">
         <v>120.3159899157367</v>
@@ -21733,10 +21733,10 @@
         <v>21.45</v>
       </c>
       <c r="I497">
-        <v>24.3</v>
+        <v>26.3</v>
       </c>
       <c r="J497">
-        <v>467</v>
+        <v>489</v>
       </c>
       <c r="K497">
         <v>108.7187906729912</v>
@@ -21776,10 +21776,10 @@
         <v>17.07</v>
       </c>
       <c r="I498">
-        <v>22.1</v>
+        <v>24.1</v>
       </c>
       <c r="J498">
-        <v>394</v>
+        <v>416</v>
       </c>
       <c r="K498">
         <v>108.0356911888938</v>
@@ -21819,10 +21819,10 @@
         <v>22.02</v>
       </c>
       <c r="I499">
-        <v>25.7</v>
+        <v>27.7</v>
       </c>
       <c r="J499">
-        <v>621</v>
+        <v>643</v>
       </c>
       <c r="K499">
         <v>127.5982440224428</v>
@@ -21862,10 +21862,10 @@
         <v>16.01</v>
       </c>
       <c r="I500">
-        <v>23.4</v>
+        <v>25.4</v>
       </c>
       <c r="J500">
-        <v>443</v>
+        <v>465</v>
       </c>
       <c r="K500">
         <v>84.3010778198571</v>

</xml_diff>